<commit_message>
converted ped presentation to images for posting on lab notebook
</commit_message>
<xml_diff>
--- a/Data/Outplant-Data2.xlsx
+++ b/Data/Outplant-Data2.xlsx
@@ -102,7 +102,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -190,7 +190,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="32">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -444,11 +444,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="10"/>
-        <c:axId val="2144607784"/>
-        <c:axId val="2144934008"/>
+        <c:axId val="-2144004088"/>
+        <c:axId val="-2144000968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144607784"/>
+        <c:axId val="-2144004088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -457,7 +457,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144934008"/>
+        <c:crossAx val="-2144000968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -465,7 +465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144934008"/>
+        <c:axId val="-2144000968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="7.0"/>
@@ -523,7 +523,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144607784"/>
+        <c:crossAx val="-2144004088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -765,11 +765,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="40"/>
-        <c:axId val="-2144795960"/>
-        <c:axId val="-2146917640"/>
+        <c:axId val="-2144105080"/>
+        <c:axId val="-2144109048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2144795960"/>
+        <c:axId val="-2144105080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -779,7 +779,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146917640"/>
+        <c:crossAx val="-2144109048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -787,7 +787,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2146917640"/>
+        <c:axId val="-2144109048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,7 +798,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144795960"/>
+        <c:crossAx val="-2144105080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -938,7 +938,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-0.0138888888888889"/>
-                  <c:y val="-8.48755627201333E-17"/>
+                  <c:y val="-8.48755627201334E-17"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1047,11 +1047,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="40"/>
-        <c:axId val="-2142632216"/>
-        <c:axId val="-2143567848"/>
+        <c:axId val="-2144149592"/>
+        <c:axId val="-2144176904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2142632216"/>
+        <c:axId val="-2144149592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1061,7 +1061,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143567848"/>
+        <c:crossAx val="-2144176904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1069,7 +1069,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143567848"/>
+        <c:axId val="-2144176904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="7.0"/>
@@ -1081,7 +1081,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142632216"/>
+        <c:crossAx val="-2144149592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -1519,8 +1519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="F23" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>